<commit_message>
Fix: template and rules validation on mhs and dosen import
</commit_message>
<xml_diff>
--- a/public/template-excel/template-import-data-master-dosen.xlsx
+++ b/public/template-excel/template-import-data-master-dosen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramadhanabdulaziz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramadhanabdulaziz/Documents/Magang/talentern/public/template-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC58699A-D904-5D4C-9FCF-20333195A95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C528AF4F-9D00-DF4F-B1E8-C001558C07E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dosen" sheetId="1" r:id="rId1"/>
@@ -906,7 +906,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1376,6 +1376,7 @@
       <c r="K28" s="29"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="yPIJlLBDK7G3QRWiTqDPMGE5aO0db/ULj2LCs9bY5vhfBM8mXYNX19iPsZEPdnOVofU4O404X5K/Po+5+EsvpQ==" saltValue="/yziWO6OVNCuQP8Esj/yww==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
     <mergeCell ref="G15:K15"/>
     <mergeCell ref="G16:K16"/>

</xml_diff>